<commit_message>
Suit xlsx file checkin
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Suite.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Suite.xlsx
@@ -1,6 +1,28 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="2370" windowWidth="8655" windowHeight="2880"/>
+  </bookViews>
+  <sheets>
+    <sheet name="FullSuite" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+  </sheets>
+  <calcPr calcId="0"/>
+</workbook>
+</file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="238">
   <si>
     <t>Description</t>
   </si>
@@ -689,10 +711,31 @@
     <t>Payroll Suite TaxWeek1CSBRNTK50PercentRegulatory201819</t>
   </si>
   <si>
-    <t>Payroll Suite TaxGeneralAndLargeTaxcodeMonthly201819</t>
-  </si>
-  <si>
-    <t>Payroll Suite TaxGeneralAndLargeTaxcodeWeekly201819</t>
+    <t>Payroll Suite TaxMonth2CSBRNTK50PercentRegulatory201819</t>
+  </si>
+  <si>
+    <t>Payroll Suite TaxMonth3CSBRNTK50PercentRegulatory201819</t>
+  </si>
+  <si>
+    <t>Payroll Suite TaxMonth4CSBRNTK50PercentRegulatory201819</t>
+  </si>
+  <si>
+    <t>Payroll Suite TaxMonth5CSBRNTK50PercentRegulatory201819</t>
+  </si>
+  <si>
+    <t>Payroll Suite TaxMonth6CSBRNTK50PercentRegulatory201819</t>
+  </si>
+  <si>
+    <t>Payroll Suite TaxMonth7CSBRNTK50PercentRegulatory201819</t>
+  </si>
+  <si>
+    <t>Payroll Suite TaxMonth8CSBRNTK50PercentRegulatory201819</t>
+  </si>
+  <si>
+    <t>Payroll Suite TaxMonth9CSBRNTK50PercentRegulatory201819</t>
+  </si>
+  <si>
+    <t>Payroll Suite TaxMonth10CSBRNTK50PercentRegulatory201819</t>
   </si>
 </sst>
 </file>
@@ -851,4 +894,2627 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D204"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="A204" sqref="A204"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="67.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>96</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>97</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>98</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>100</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>103</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>106</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>107</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>109</v>
+      </c>
+      <c r="B94" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>111</v>
+      </c>
+      <c r="B95" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>112</v>
+      </c>
+      <c r="B97" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>113</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>115</v>
+      </c>
+      <c r="B99" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>116</v>
+      </c>
+      <c r="B100" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>121</v>
+      </c>
+      <c r="B101" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>123</v>
+      </c>
+      <c r="B102" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>125</v>
+      </c>
+      <c r="B103" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>126</v>
+      </c>
+      <c r="B104" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>128</v>
+      </c>
+      <c r="B105" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>130</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>131</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B115" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B116" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B117" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="B118" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B119" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B120" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B121" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B122" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B123" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B124" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B125" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B126" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B127" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B128" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>188</v>
+      </c>
+      <c r="B136" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B137" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B138" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B140" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B143" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B144" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B145" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B146" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B147" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B148" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B149" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B150" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B151" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B152" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B153" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B154" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B155" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B156" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="B157" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B158" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>197</v>
+      </c>
+      <c r="B171" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>198</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>199</v>
+      </c>
+      <c r="B173" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>200</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>201</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>202</v>
+      </c>
+      <c r="B176" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>203</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>204</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>206</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>208</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>209</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>210</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>212</v>
+      </c>
+      <c r="B183" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>214</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>215</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>216</v>
+      </c>
+      <c r="B186" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>218</v>
+      </c>
+      <c r="B187" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>219</v>
+      </c>
+      <c r="B188" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>220</v>
+      </c>
+      <c r="B189" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>222</v>
+      </c>
+      <c r="B190" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>223</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>221</v>
+      </c>
+      <c r="B192" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>224</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>225</v>
+      </c>
+      <c r="B194" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>228</v>
+      </c>
+      <c r="B195" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>229</v>
+      </c>
+      <c r="B196" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>230</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>231</v>
+      </c>
+      <c r="B198" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>232</v>
+      </c>
+      <c r="B199" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>233</v>
+      </c>
+      <c r="B200" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>234</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>235</v>
+      </c>
+      <c r="B202" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>236</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>237</v>
+      </c>
+      <c r="B204" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
uploaded the suite xlsx file dtd april 13 2018
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Suite.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Suite.xlsx
@@ -1,3 +1,26 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Automation metrix template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F1B2C38B-ED54-4F2F-AFB8-17C71A5B334F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="FullSuite" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+  </sheets>
+  <calcPr calcId="0"/>
+</workbook>
+</file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="326">
@@ -1189,4 +1212,3408 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D275"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="I268" sqref="I268"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="67.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>96</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>97</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>98</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>100</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>103</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>106</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>107</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>109</v>
+      </c>
+      <c r="B94" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>111</v>
+      </c>
+      <c r="B95" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>112</v>
+      </c>
+      <c r="B97" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>113</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>115</v>
+      </c>
+      <c r="B99" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>116</v>
+      </c>
+      <c r="B100" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>121</v>
+      </c>
+      <c r="B101" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>123</v>
+      </c>
+      <c r="B102" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>125</v>
+      </c>
+      <c r="B103" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>126</v>
+      </c>
+      <c r="B104" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>128</v>
+      </c>
+      <c r="B105" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>130</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>131</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B115" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B116" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B117" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="B118" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B119" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B120" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B121" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B122" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B123" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B124" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B125" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B126" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B127" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B128" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>188</v>
+      </c>
+      <c r="B136" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B137" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B138" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B140" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B143" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B144" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B145" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B146" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B147" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B148" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B149" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B150" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B151" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B152" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B153" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B154" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B155" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B156" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="B157" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B158" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B171" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B172" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B173" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B174" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B175" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B176" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B177" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A178" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="B178" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="B179" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="B180" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="B181" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="B182" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="B183" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="B184" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="B185" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="B186" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="C186" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="B187" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="C187" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="B188" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="C188" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="B189" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="C189" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="B190" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="C190" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="B191" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="C191" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="B192" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="C192" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B193" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="C193" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A194" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B194" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C194" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A195" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B195" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C195" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A196" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B196" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C196" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A197" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B197" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C197" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A198" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B198" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C198" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A199" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B199" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C199" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A200" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B200" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C200" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A201" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B201" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C201" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A202" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B202" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C202" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A203" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B203" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C203" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A204" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="B204" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C204" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A205" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="B205" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C205" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A206" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="B206" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C206" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A207" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="B207" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C207" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A208" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="B208" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C208" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A209" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="B209" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C209" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A210" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="B210" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C210" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A211" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="B211" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C211" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A212" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="B212" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C212" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A213" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="B213" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C213" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="B214" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="C214" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="B215" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="C215" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B216" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C216" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B217" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B218" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B219" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B220" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B221" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B222" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="B223" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="B224" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B225" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="B226" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="B227" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="B228" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="B229" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B230" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B231" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B232" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B233" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B234" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B235" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B236" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B237" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B238" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B239" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B240" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B241" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B242" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B243" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B244" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C244" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B245" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C245" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B246" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C246" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A247" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B247" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C247" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A248" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B248" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C248" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A249" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B249" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C249" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A250" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B250" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="C250" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A251" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B251" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="C251" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A252" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B252" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="C252" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A253" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B253" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="C253" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A254" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B254" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="C254" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A255" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B255" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="C255" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A256" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B256" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C256" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A257" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B257" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C257" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A258" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B258" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C258" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A259" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B259" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C259" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A260" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="B260" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C260" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A261" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="B261" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C261" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A262" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="B262" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C262" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A263" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B263" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C263" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A264" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="B264" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C264" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A265" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="B265" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C265" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A266" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B266" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C266" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A267" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="B267" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C267" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A268" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="B268" s="29" t="s">
+        <v>316</v>
+      </c>
+      <c r="C268" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A269" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="B269" s="29" t="s">
+        <v>318</v>
+      </c>
+      <c r="C269" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A270" s="28" t="s">
+        <v>319</v>
+      </c>
+      <c r="B270" s="29" t="s">
+        <v>320</v>
+      </c>
+      <c r="C270" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" s="28" t="s">
+        <v>321</v>
+      </c>
+      <c r="B271" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" s="28" t="s">
+        <v>322</v>
+      </c>
+      <c r="B272" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" s="28" t="s">
+        <v>323</v>
+      </c>
+      <c r="B273" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" s="28" t="s">
+        <v>324</v>
+      </c>
+      <c r="B274" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="B275" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modification done for courtOrder Scenario two functionality
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Suite.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Suite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5760E3C9-5528-4CDE-A484-290EFF9F52C9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{193B7C30-8409-4825-9E16-E262BF55AFC3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="329">
   <si>
     <t>Description</t>
   </si>
@@ -1007,6 +1007,9 @@
   </si>
   <si>
     <t>Payroll Suite CourtOrder AEO1971civildebt201819</t>
+  </si>
+  <si>
+    <t>Payroll Suite CourtOrder CAEO1971civildebt201819</t>
   </si>
 </sst>
 </file>
@@ -1551,10 +1554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D276"/>
+  <dimension ref="A1:D277"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="A281" sqref="A281"/>
+      <selection activeCell="B282" sqref="B282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4600,6 +4603,17 @@
         <v>326</v>
       </c>
       <c r="C276" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>328</v>
+      </c>
+      <c r="B277" s="35" t="s">
+        <v>326</v>
+      </c>
+      <c r="C277" s="2" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
committing files for 3d scenarios
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Suite.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Suite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1D2DB23C-BCB6-45CA-A60C-68A426DF67CB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3CB899EB-A62E-42EC-8B7D-A8654C8184F3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1566,7 +1566,7 @@
   <dimension ref="A1:D278"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="B279" sqref="B279"/>
+      <selection activeCell="F275" sqref="F275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4616,7 +4616,7 @@
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
+      <c r="A277" s="34" t="s">
         <v>327</v>
       </c>
       <c r="B277" s="35" t="s">
@@ -4627,7 +4627,7 @@
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
+      <c r="A278" s="34" t="s">
         <v>328</v>
       </c>
       <c r="B278" s="35" t="s">

</xml_diff>

<commit_message>
working for scenario 5
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Suite.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Suite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E614C5DA-3D4A-40F7-B270-A110C6032802}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D3531777-07E0-4AF2-9280-1F74525BA605}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="334">
   <si>
     <t>Description</t>
   </si>
@@ -1022,6 +1022,9 @@
   </si>
   <si>
     <t>Payroll Suite CourtOrder PAEO1971Maintenance201819</t>
+  </si>
+  <si>
+    <t>Payroll Suite CourtOrder PAEO1971Fine201819</t>
   </si>
 </sst>
 </file>
@@ -1566,10 +1569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D279"/>
+  <dimension ref="A1:D280"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="B282" sqref="B282"/>
+      <selection activeCell="A282" sqref="A282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4648,6 +4651,17 @@
         <v>331</v>
       </c>
       <c r="C279" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" s="34" t="s">
+        <v>333</v>
+      </c>
+      <c r="B280" s="35" t="s">
+        <v>331</v>
+      </c>
+      <c r="C280" s="2" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>